<commit_message>
Add balance de comprobacion Objects
</commit_message>
<xml_diff>
--- a/Contabilidad.xlsx
+++ b/Contabilidad.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2543" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4277" uniqueCount="255">
   <si>
     <t>Libro Diario</t>
   </si>
@@ -836,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="261">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -880,6 +880,321 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -3075,7 +3390,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="121">
+      <c r="A1" t="s" s="226">
         <v>176</v>
       </c>
     </row>
@@ -3290,7 +3605,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="122">
+      <c r="A17" t="s" s="227">
         <v>176</v>
       </c>
     </row>
@@ -3385,7 +3700,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="123">
+      <c r="A27" t="s" s="228">
         <v>176</v>
       </c>
     </row>
@@ -3680,7 +3995,7 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s" s="124">
+      <c r="A47" t="s" s="229">
         <v>176</v>
       </c>
     </row>
@@ -3795,7 +4110,7 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s" s="125">
+      <c r="A58" t="s" s="230">
         <v>176</v>
       </c>
     </row>
@@ -3970,7 +4285,7 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="s" s="126">
+      <c r="A72" t="s" s="231">
         <v>176</v>
       </c>
     </row>
@@ -4045,7 +4360,7 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="s" s="127">
+      <c r="A81" t="s" s="232">
         <v>176</v>
       </c>
     </row>
@@ -4260,7 +4575,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="s" s="128">
+      <c r="A97" t="s" s="233">
         <v>176</v>
       </c>
     </row>
@@ -4311,7 +4626,7 @@
         <v>300.0</v>
       </c>
       <c r="F101" t="n">
-        <v>-300.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="102">
@@ -4335,7 +4650,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="s" s="129">
+      <c r="A106" t="s" s="234">
         <v>176</v>
       </c>
     </row>
@@ -4410,7 +4725,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="s" s="130">
+      <c r="A115" t="s" s="235">
         <v>176</v>
       </c>
     </row>
@@ -4461,7 +4776,7 @@
         <v>112.5</v>
       </c>
       <c r="F119" t="n">
-        <v>-112.5</v>
+        <v>112.5</v>
       </c>
     </row>
     <row r="120">
@@ -4485,7 +4800,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="s" s="131">
+      <c r="A124" t="s" s="236">
         <v>176</v>
       </c>
     </row>
@@ -4560,7 +4875,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="s" s="132">
+      <c r="A133" t="s" s="237">
         <v>176</v>
       </c>
     </row>
@@ -4611,7 +4926,7 @@
         <v>624.94</v>
       </c>
       <c r="F137" t="n">
-        <v>-624.94</v>
+        <v>624.94</v>
       </c>
     </row>
     <row r="138">
@@ -4635,7 +4950,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="s" s="133">
+      <c r="A142" t="s" s="238">
         <v>176</v>
       </c>
     </row>
@@ -4710,7 +5025,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="s" s="134">
+      <c r="A151" t="s" s="239">
         <v>176</v>
       </c>
     </row>
@@ -4761,7 +5076,7 @@
         <v>3500.0</v>
       </c>
       <c r="F155" t="n">
-        <v>-3500.0</v>
+        <v>3500.0</v>
       </c>
     </row>
     <row r="156">
@@ -4781,7 +5096,7 @@
         <v>33600.0</v>
       </c>
       <c r="F156" t="n">
-        <v>-37100.0</v>
+        <v>37100.0</v>
       </c>
     </row>
     <row r="157">
@@ -4805,7 +5120,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="s" s="135">
+      <c r="A161" t="s" s="240">
         <v>176</v>
       </c>
     </row>
@@ -4856,7 +5171,7 @@
         <v>487.78</v>
       </c>
       <c r="F165" t="n">
-        <v>-487.78</v>
+        <v>487.78</v>
       </c>
     </row>
     <row r="166">
@@ -4880,7 +5195,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="s" s="136">
+      <c r="A170" t="s" s="241">
         <v>176</v>
       </c>
     </row>
@@ -4931,7 +5246,7 @@
         <v>627.15</v>
       </c>
       <c r="F174" t="n">
-        <v>-627.15</v>
+        <v>627.15</v>
       </c>
     </row>
     <row r="175">
@@ -4955,7 +5270,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="s" s="137">
+      <c r="A179" t="s" s="242">
         <v>176</v>
       </c>
     </row>
@@ -5006,7 +5321,7 @@
         <v>1710.0</v>
       </c>
       <c r="F183" t="n">
-        <v>-1710.0</v>
+        <v>1710.0</v>
       </c>
     </row>
     <row r="184">
@@ -5026,7 +5341,7 @@
         <v>3450.0</v>
       </c>
       <c r="F184" t="n">
-        <v>-5160.0</v>
+        <v>5160.0</v>
       </c>
     </row>
     <row r="185">
@@ -5046,7 +5361,7 @@
         <v>0.0</v>
       </c>
       <c r="F185" t="n">
-        <v>-4410.0</v>
+        <v>5910.0</v>
       </c>
     </row>
     <row r="186">
@@ -5066,7 +5381,7 @@
         <v>2220.0</v>
       </c>
       <c r="F186" t="n">
-        <v>-6630.0</v>
+        <v>3690.0</v>
       </c>
     </row>
     <row r="187">
@@ -5086,7 +5401,7 @@
         <v>0.0</v>
       </c>
       <c r="F187" t="n">
-        <v>0.0</v>
+        <v>10320.0</v>
       </c>
     </row>
     <row r="188">
@@ -5106,11 +5421,11 @@
         <v>7380.0</v>
       </c>
       <c r="F188" t="n">
-        <v>0.0</v>
+        <v>10320.0</v>
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="s" s="138">
+      <c r="A192" t="s" s="243">
         <v>176</v>
       </c>
     </row>
@@ -5161,7 +5476,7 @@
         <v>55.0</v>
       </c>
       <c r="F196" t="n">
-        <v>-55.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="197">
@@ -5185,7 +5500,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="s" s="139">
+      <c r="A201" t="s" s="244">
         <v>176</v>
       </c>
     </row>
@@ -5236,7 +5551,7 @@
         <v>1857.6</v>
       </c>
       <c r="F205" t="n">
-        <v>-1857.6</v>
+        <v>1857.6</v>
       </c>
     </row>
     <row r="206">
@@ -5260,7 +5575,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" t="s" s="140">
+      <c r="A210" t="s" s="245">
         <v>176</v>
       </c>
     </row>
@@ -5311,7 +5626,7 @@
         <v>1500.0</v>
       </c>
       <c r="F214" t="n">
-        <v>-1500.0</v>
+        <v>1500.0</v>
       </c>
     </row>
     <row r="215">
@@ -5335,7 +5650,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="s" s="141">
+      <c r="A219" t="s" s="246">
         <v>176</v>
       </c>
     </row>
@@ -5386,7 +5701,7 @@
         <v>118500.0</v>
       </c>
       <c r="F223" t="n">
-        <v>-118500.0</v>
+        <v>118500.0</v>
       </c>
     </row>
     <row r="224">
@@ -5410,7 +5725,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" t="s" s="142">
+      <c r="A228" t="s" s="247">
         <v>176</v>
       </c>
     </row>
@@ -5461,7 +5776,7 @@
         <v>14250.0</v>
       </c>
       <c r="F232" t="n">
-        <v>-14250.0</v>
+        <v>14250.0</v>
       </c>
     </row>
     <row r="233">
@@ -5481,7 +5796,7 @@
         <v>28750.0</v>
       </c>
       <c r="F233" t="n">
-        <v>-43000.0</v>
+        <v>43000.0</v>
       </c>
     </row>
     <row r="234">
@@ -5501,7 +5816,7 @@
         <v>0.0</v>
       </c>
       <c r="F234" t="n">
-        <v>-36750.0</v>
+        <v>49250.0</v>
       </c>
     </row>
     <row r="235">
@@ -5521,7 +5836,7 @@
         <v>18500.0</v>
       </c>
       <c r="F235" t="n">
-        <v>-55250.0</v>
+        <v>30750.0</v>
       </c>
     </row>
     <row r="236">
@@ -5541,11 +5856,11 @@
         <v>61500.0</v>
       </c>
       <c r="F236" t="n">
-        <v>55250.0</v>
+        <v>30750.0</v>
       </c>
     </row>
     <row r="240">
-      <c r="A240" t="s" s="143">
+      <c r="A240" t="s" s="248">
         <v>176</v>
       </c>
     </row>
@@ -5640,7 +5955,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" t="s" s="144">
+      <c r="A250" t="s" s="249">
         <v>176</v>
       </c>
     </row>
@@ -5715,7 +6030,7 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" t="s" s="145">
+      <c r="A259" t="s" s="250">
         <v>176</v>
       </c>
     </row>
@@ -5790,7 +6105,7 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" t="s" s="146">
+      <c r="A268" t="s" s="251">
         <v>176</v>
       </c>
     </row>
@@ -5865,7 +6180,7 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" t="s" s="147">
+      <c r="A277" t="s" s="252">
         <v>176</v>
       </c>
     </row>
@@ -5940,7 +6255,7 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" t="s" s="148">
+      <c r="A286" t="s" s="253">
         <v>176</v>
       </c>
     </row>
@@ -6015,7 +6330,7 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" t="s" s="149">
+      <c r="A295" t="s" s="254">
         <v>176</v>
       </c>
     </row>
@@ -6090,7 +6405,7 @@
       </c>
     </row>
     <row r="304">
-      <c r="A304" t="s" s="150">
+      <c r="A304" t="s" s="255">
         <v>176</v>
       </c>
     </row>
@@ -6165,7 +6480,7 @@
       </c>
     </row>
     <row r="313">
-      <c r="A313" t="s" s="151">
+      <c r="A313" t="s" s="256">
         <v>176</v>
       </c>
     </row>
@@ -6240,7 +6555,7 @@
       </c>
     </row>
     <row r="322">
-      <c r="A322" t="s" s="152">
+      <c r="A322" t="s" s="257">
         <v>176</v>
       </c>
     </row>
@@ -6315,7 +6630,7 @@
       </c>
     </row>
     <row r="331">
-      <c r="A331" t="s" s="153">
+      <c r="A331" t="s" s="258">
         <v>176</v>
       </c>
     </row>
@@ -6390,7 +6705,7 @@
       </c>
     </row>
     <row r="340">
-      <c r="A340" t="s" s="154">
+      <c r="A340" t="s" s="259">
         <v>176</v>
       </c>
     </row>
@@ -6465,7 +6780,7 @@
       </c>
     </row>
     <row r="349">
-      <c r="A349" t="s" s="155">
+      <c r="A349" t="s" s="260">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Separate file creation from ciclo contable
</commit_message>
<xml_diff>
--- a/Contabilidad.xlsx
+++ b/Contabilidad.xlsx
@@ -128,15 +128,15 @@
     <t>DEPRECIACION ACUMULADA MUEBLES DE OFICINA</t>
   </si>
   <si>
+    <t>1.2.03</t>
+  </si>
+  <si>
+    <t>EQUIPO DE COMPUTO</t>
+  </si>
+  <si>
     <t>Clientes</t>
   </si>
   <si>
-    <t>1.2.03</t>
-  </si>
-  <si>
-    <t>EQUIPO DE COMPUTO</t>
-  </si>
-  <si>
     <t>1.2.04</t>
   </si>
   <si>
@@ -206,24 +206,30 @@
     <t>2.2</t>
   </si>
   <si>
+    <t>Equipo de computo</t>
+  </si>
+  <si>
     <t>PASIVO NO CORRIENTE</t>
   </si>
   <si>
     <t>2.2.01</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
     <t>PRESTAMOS BANCARIOS LARGO PLAZO</t>
   </si>
   <si>
+    <t>Proveedores</t>
+  </si>
+  <si>
     <t>3.</t>
   </si>
   <si>
     <t>PATRIMONIO</t>
   </si>
   <si>
-    <t>Equipo de computo</t>
-  </si>
-  <si>
     <t>3.1.</t>
   </si>
   <si>
@@ -233,52 +239,70 @@
     <t>3.1.01</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
     <t>CAPITAL</t>
   </si>
   <si>
-    <t>Proveedores</t>
+    <t>Prestamos bancarios largo plazo</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>El estado de situacion inicial</t>
+  </si>
+  <si>
+    <t>Junio 02</t>
+  </si>
+  <si>
+    <t>Bancos</t>
+  </si>
+  <si>
+    <t>Apertura cuenta corriente No deposito en efectivo</t>
+  </si>
+  <si>
+    <t>Ventas</t>
+  </si>
+  <si>
+    <t>IVA ventas</t>
   </si>
   <si>
     <t>Estado de Resultado Integral</t>
   </si>
   <si>
-    <t>Prestamos bancarios largo plazo</t>
+    <t>Venta mercaderias segun factura No</t>
+  </si>
+  <si>
+    <t>Costo de venta</t>
   </si>
   <si>
     <t>4.</t>
   </si>
   <si>
-    <t>Capital</t>
-  </si>
-  <si>
     <t>INGRESOS</t>
   </si>
   <si>
     <t>4.1</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>INGRESOS OPERACIONALES</t>
   </si>
   <si>
-    <t>El estado de situacion inicial</t>
+    <t>Venta de mercaderia precio de costo</t>
   </si>
   <si>
     <t>4.1.01</t>
   </si>
   <si>
-    <t>Junio 02</t>
-  </si>
-  <si>
     <t>VENTAS</t>
   </si>
   <si>
-    <t>Bancos</t>
+    <t>Deposito de la venta realizada</t>
+  </si>
+  <si>
+    <t>Junio 05</t>
   </si>
   <si>
     <t>5.</t>
@@ -287,22 +311,22 @@
     <t>GASTOS</t>
   </si>
   <si>
-    <t>Apertura cuenta corriente No deposito en efectivo</t>
-  </si>
-  <si>
     <t>5.1</t>
   </si>
   <si>
     <t>GASTOS OPERACIONALES</t>
   </si>
   <si>
+    <t>Contratacion de una poliza al 2.5% mensual</t>
+  </si>
+  <si>
     <t>5.1.01</t>
   </si>
   <si>
     <t>SUELDOS Y SALARIOS</t>
   </si>
   <si>
-    <t>Ventas</t>
+    <t>Arriendos</t>
   </si>
   <si>
     <t>5.1.02</t>
@@ -311,7 +335,7 @@
     <t>ARRIENDOS</t>
   </si>
   <si>
-    <t>IVA ventas</t>
+    <t>IVA compras</t>
   </si>
   <si>
     <t>5.1.03</t>
@@ -323,16 +347,16 @@
     <t>5.1.04</t>
   </si>
   <si>
-    <t>Venta mercaderias segun factura No</t>
-  </si>
-  <si>
     <t>GASTOS DEPRECIACION MUEBLES DE OFICINA</t>
   </si>
   <si>
+    <t>Arriendo</t>
+  </si>
+  <si>
     <t>5.1.05</t>
   </si>
   <si>
-    <t>Costo de venta</t>
+    <t>Caja Chica</t>
   </si>
   <si>
     <t>GASTOS DEPRECIACION EQUIPO DE COMPUTO</t>
@@ -350,7 +374,7 @@
     <t>Decimo Cuarto</t>
   </si>
   <si>
-    <t>Venta de mercaderia precio de costo</t>
+    <t>Apertura de fondo de caja chica con cheque No 002</t>
   </si>
   <si>
     <t>5.1.08</t>
@@ -359,6 +383,9 @@
     <t>Fondos de Reserva</t>
   </si>
   <si>
+    <t>Junio 06</t>
+  </si>
+  <si>
     <t>5.1.09</t>
   </si>
   <si>
@@ -377,45 +404,30 @@
     <t>Horas extra</t>
   </si>
   <si>
-    <t>Deposito de la venta realizada</t>
-  </si>
-  <si>
-    <t>Junio 05</t>
-  </si>
-  <si>
-    <t>Contratacion de una poliza al 2.5% mensual</t>
-  </si>
-  <si>
-    <t>Arriendos</t>
-  </si>
-  <si>
-    <t>IVA compras</t>
-  </si>
-  <si>
-    <t>Arriendo</t>
-  </si>
-  <si>
-    <t>Caja Chica</t>
-  </si>
-  <si>
-    <t>Apertura de fondo de caja chica con cheque No 002</t>
-  </si>
-  <si>
-    <t>Junio 06</t>
-  </si>
-  <si>
     <t>Compra de mercaderia</t>
   </si>
   <si>
+    <t>Junio 07</t>
+  </si>
+  <si>
+    <t>Transporte y movilizacion</t>
+  </si>
+  <si>
+    <t>Pago transporte Guayaquil</t>
+  </si>
+  <si>
+    <t>Junio 09</t>
+  </si>
+  <si>
+    <t>Devolucion 5 impresoras por estar en mal estado de la compra 6 de junio</t>
+  </si>
+  <si>
+    <t>Junio 10</t>
+  </si>
+  <si>
     <t>5.1.12</t>
   </si>
   <si>
-    <t>Junio 07</t>
-  </si>
-  <si>
-    <t>Transporte y movilizacion</t>
-  </si>
-  <si>
     <t>5.1.13</t>
   </si>
   <si>
@@ -425,6 +437,9 @@
     <t>5.1.14</t>
   </si>
   <si>
+    <t>Venta de computadoras</t>
+  </si>
+  <si>
     <t>Honorarios</t>
   </si>
   <si>
@@ -434,37 +449,22 @@
     <t>Impuestos Fiscales</t>
   </si>
   <si>
-    <t>Pago transporte Guayaquil</t>
-  </si>
-  <si>
-    <t>Junio 09</t>
-  </si>
-  <si>
-    <t>Devolucion 5 impresoras por estar en mal estado de la compra 6 de junio</t>
-  </si>
-  <si>
-    <t>Junio 10</t>
+    <t>Registro precio de costo</t>
+  </si>
+  <si>
+    <t>Junio 12</t>
+  </si>
+  <si>
+    <t>Devolucion ventas</t>
   </si>
   <si>
     <t>GASTOS NO OPERACIONALES</t>
   </si>
   <si>
-    <t>Venta de computadoras</t>
-  </si>
-  <si>
     <t>5.2.01</t>
   </si>
   <si>
     <t>Costo de Venta</t>
-  </si>
-  <si>
-    <t>Registro precio de costo</t>
-  </si>
-  <si>
-    <t>Junio 12</t>
-  </si>
-  <si>
-    <t>Devolucion ventas</t>
   </si>
   <si>
     <t>Devolucion ventas a precio de costo</t>
@@ -877,10 +877,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -1033,7 +1033,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="26" customWidth="true" width="7.63" collapsed="true"/>
+    <col min="1" max="26" customWidth="true" width="7.63" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1168,10 +1168,10 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23">
@@ -1271,72 +1271,72 @@
         <v>63</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="4"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47">
@@ -1345,138 +1345,138 @@
     </row>
     <row r="48">
       <c r="A48" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="4" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="4" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="4" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="4" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="4" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="4" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="4" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66">
@@ -1484,15 +1484,15 @@
         <v>5.2</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70">
@@ -1520,7 +1520,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="26" customWidth="true" width="7.63" collapsed="true"/>
+    <col min="1" max="26" customWidth="true" width="7.63" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1559,7 +1559,7 @@
     <row r="4">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6">
@@ -1595,7 +1595,7 @@
     </row>
     <row r="7">
       <c r="B7" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D7" s="7">
         <v>25000.0</v>
@@ -1608,23 +1608,23 @@
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E8" s="7">
         <v>3500.0</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9">
       <c r="C9" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E9" s="7">
         <v>1500.0</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="10">
       <c r="C10" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E10" s="7">
         <v>118500.0</v>
@@ -1640,18 +1640,18 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D12" s="7">
         <v>15000.0</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>13</v>
@@ -1670,15 +1670,15 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>13</v>
@@ -1689,10 +1689,10 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E16" s="7">
         <v>14250.0</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="17">
       <c r="C17" s="7" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E17" s="7">
         <v>1710.0</v>
@@ -1708,18 +1708,18 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D19" s="7">
         <v>7250.0</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="20">
       <c r="A20" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>27</v>
@@ -1738,18 +1738,18 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D22" s="7">
         <v>15960.0</v>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>13</v>
@@ -1768,15 +1768,15 @@
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>44</v>
@@ -1787,10 +1787,10 @@
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E26" s="7">
         <v>5000.0</v>
@@ -1798,18 +1798,18 @@
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="D28" s="7">
         <v>200.0</v>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="29">
       <c r="B29" s="7" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D29" s="7">
         <v>24.0</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="30">
       <c r="A30" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E30" s="7">
         <v>224.0</v>
@@ -1836,18 +1836,18 @@
     </row>
     <row r="31">
       <c r="A31" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="7" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D32" s="7">
         <v>100.0</v>
@@ -1855,10 +1855,10 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E33" s="7">
         <v>100.0</v>
@@ -1866,15 +1866,15 @@
     </row>
     <row r="34">
       <c r="A34" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>27</v>
@@ -1885,7 +1885,7 @@
     </row>
     <row r="36">
       <c r="B36" s="7" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D36" s="7">
         <v>1320.0</v>
@@ -1893,10 +1893,10 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E37" s="7">
         <v>12320.0</v>
@@ -1904,7 +1904,7 @@
     </row>
     <row r="38">
       <c r="A38" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>130</v>
@@ -1912,10 +1912,10 @@
     </row>
     <row r="39">
       <c r="A39" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="D39" s="7">
         <v>100.0</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="40">
       <c r="A40" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>13</v>
@@ -1934,15 +1934,15 @@
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>13</v>
@@ -1953,7 +1953,7 @@
     </row>
     <row r="43">
       <c r="A43" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>27</v>
@@ -1964,7 +1964,7 @@
     </row>
     <row r="44">
       <c r="C44" s="7" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="E44" s="7">
         <v>180.0</v>
@@ -1972,18 +1972,18 @@
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D46" s="7">
         <v>28750.0</v>
@@ -2001,10 +2001,10 @@
     </row>
     <row r="48">
       <c r="A48" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E48" s="7">
         <v>28750.0</v>
@@ -2012,7 +2012,7 @@
     </row>
     <row r="49">
       <c r="C49" s="7" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E49" s="7">
         <v>3450.0</v>
@@ -2020,18 +2020,18 @@
     </row>
     <row r="50">
       <c r="A50" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D51" s="7">
         <v>14245.2</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="52">
       <c r="A52" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>27</v>
@@ -2050,18 +2050,18 @@
     </row>
     <row r="53">
       <c r="A53" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="D54" s="7">
         <v>6250.0</v>
@@ -2069,7 +2069,7 @@
     </row>
     <row r="55">
       <c r="B55" s="7" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D55" s="7">
         <v>750.0</v>
@@ -2077,10 +2077,10 @@
     </row>
     <row r="56">
       <c r="A56" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E56" s="7">
         <v>6250.0</v>
@@ -2096,15 +2096,15 @@
     </row>
     <row r="58">
       <c r="A58" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>27</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="60">
       <c r="A60" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E60" s="7">
         <v>3103.8</v>
@@ -2126,7 +2126,7 @@
     </row>
     <row r="61">
       <c r="A61" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>151</v>
@@ -2134,7 +2134,7 @@
     </row>
     <row r="62">
       <c r="A62" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>152</v>
@@ -2145,10 +2145,10 @@
     </row>
     <row r="63">
       <c r="A63" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E63" s="7">
         <v>300.0</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="64">
       <c r="A64" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>153</v>
@@ -2164,10 +2164,10 @@
     </row>
     <row r="65">
       <c r="A65" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D65" s="7">
         <v>500.0</v>
@@ -2175,10 +2175,10 @@
     </row>
     <row r="66">
       <c r="A66" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E66" s="7">
         <v>500.0</v>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="67">
       <c r="A67" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>154</v>
@@ -2205,7 +2205,7 @@
     </row>
     <row r="69">
       <c r="B69" s="7" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7">
@@ -2214,7 +2214,7 @@
     </row>
     <row r="70">
       <c r="A70" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>157</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="71">
       <c r="A71" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>158</v>
@@ -2244,10 +2244,10 @@
     </row>
     <row r="73">
       <c r="A73" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E73" s="7">
         <v>300.0</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="74">
       <c r="A74" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>160</v>
@@ -2274,7 +2274,7 @@
     </row>
     <row r="76">
       <c r="B76" s="7" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D76" s="7">
         <v>3600.0</v>
@@ -2282,10 +2282,10 @@
     </row>
     <row r="77">
       <c r="A77" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E77" s="7">
         <v>33600.0</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="78">
       <c r="A78" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>130</v>
@@ -2304,7 +2304,7 @@
         <v>162</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D79" s="7">
         <v>300.0</v>
@@ -2312,10 +2312,10 @@
     </row>
     <row r="80">
       <c r="A80" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E80" s="7">
         <v>300.0</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="81">
       <c r="A81" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>163</v>
@@ -2334,7 +2334,7 @@
         <v>164</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D82" s="7">
         <v>20720.0</v>
@@ -2342,10 +2342,10 @@
     </row>
     <row r="83">
       <c r="A83" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E83" s="7">
         <v>18500.0</v>
@@ -2353,7 +2353,7 @@
     </row>
     <row r="84">
       <c r="C84" s="7" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E84" s="7">
         <v>2220.0</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="85">
       <c r="A85" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>165</v>
@@ -2372,7 +2372,7 @@
         <v>164</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="D86" s="7">
         <v>9157.07</v>
@@ -2380,7 +2380,7 @@
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C87" s="7" t="s">
         <v>27</v>
@@ -2391,7 +2391,7 @@
     </row>
     <row r="88">
       <c r="A88" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>166</v>
@@ -2402,7 +2402,7 @@
         <v>167</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D89" s="7">
         <v>14850.0</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="90">
       <c r="B90" s="7" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="D90" s="7">
         <v>150.0</v>
@@ -2418,10 +2418,10 @@
     </row>
     <row r="91">
       <c r="A91" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E91" s="7">
         <v>15000.0</v>
@@ -2429,7 +2429,7 @@
     </row>
     <row r="92">
       <c r="A92" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>168</v>
@@ -2440,7 +2440,7 @@
         <v>167</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D93" s="7">
         <v>112.5</v>
@@ -2448,7 +2448,7 @@
     </row>
     <row r="94">
       <c r="B94" s="14" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D94" s="7">
         <v>624.94</v>
@@ -2456,7 +2456,7 @@
     </row>
     <row r="95">
       <c r="A95" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>37</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="97">
       <c r="A97" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>169</v>
@@ -2494,7 +2494,7 @@
     </row>
     <row r="99">
       <c r="B99" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D99" s="7">
         <v>227.5</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="100">
       <c r="B100" s="7" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D100" s="7">
         <v>430.21</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="101">
       <c r="B101" s="7" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D101" s="7">
         <v>430.14</v>
@@ -2519,7 +2519,7 @@
     <row r="102">
       <c r="A102" s="5"/>
       <c r="B102" s="3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C102" s="5"/>
       <c r="D102" s="3">
@@ -2532,16 +2532,16 @@
       <c r="B103" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C103" s="10"/>
+      <c r="C103" s="9"/>
       <c r="D103" s="15">
         <v>429.97</v>
       </c>
-      <c r="E103" s="10"/>
+      <c r="E103" s="9"/>
     </row>
     <row r="104">
       <c r="A104" s="5"/>
       <c r="B104" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="6">
@@ -2551,7 +2551,7 @@
     </row>
     <row r="105">
       <c r="A105" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B105" s="5"/>
       <c r="C105" s="3" t="s">
@@ -2568,7 +2568,7 @@
       <c r="C106" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D106" s="10"/>
+      <c r="D106" s="9"/>
       <c r="E106" s="15">
         <v>627.15</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="A109" s="5"/>
       <c r="B109" s="5"/>
       <c r="C109" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D109" s="5"/>
       <c r="E109" s="6">
@@ -2608,21 +2608,21 @@
     </row>
     <row r="110">
       <c r="A110" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B110" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
-      <c r="E110" s="10"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
     </row>
     <row r="111">
       <c r="A111" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="6">
@@ -2632,11 +2632,11 @@
     </row>
     <row r="112">
       <c r="A112" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B112" s="5"/>
       <c r="C112" s="3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="3">
@@ -2656,7 +2656,7 @@
     </row>
     <row r="114">
       <c r="A114" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B114" s="3" t="s">
         <v>173</v>
@@ -2682,9 +2682,9 @@
     <row r="117">
       <c r="A117" s="5"/>
       <c r="B117" s="5"/>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
-      <c r="E117" s="10"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
     </row>
     <row r="118">
       <c r="A118" s="5"/>
@@ -2703,9 +2703,9 @@
     <row r="120">
       <c r="A120" s="5"/>
       <c r="B120" s="5"/>
-      <c r="C120" s="10"/>
-      <c r="D120" s="10"/>
-      <c r="E120" s="10"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
     </row>
     <row r="121">
       <c r="A121" s="5"/>
@@ -2724,9 +2724,9 @@
     <row r="123">
       <c r="A123" s="5"/>
       <c r="B123" s="5"/>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="10"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
     </row>
     <row r="124">
       <c r="A124" s="5"/>
@@ -2752,9 +2752,9 @@
     <row r="127">
       <c r="A127" s="5"/>
       <c r="B127" s="5"/>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="10"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
     </row>
     <row r="128">
       <c r="A128" s="5"/>
@@ -2774,14 +2774,14 @@
       <c r="A130" s="5"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
-      <c r="D130" s="10"/>
+      <c r="D130" s="9"/>
       <c r="E130" s="8"/>
     </row>
     <row r="131">
       <c r="A131" s="5"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
-      <c r="D131" s="10"/>
+      <c r="D131" s="9"/>
       <c r="E131" s="5"/>
     </row>
   </sheetData>
@@ -2840,7 +2840,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C5" t="n">
         <v>1.0</v>
@@ -2857,10 +2857,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
@@ -2877,10 +2877,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
         <v>86</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
       </c>
       <c r="C7" t="n">
         <v>3.0</v>
@@ -2897,10 +2897,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C8" t="n">
         <v>5.0</v>
@@ -2917,10 +2917,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C9" t="n">
         <v>10.0</v>
@@ -2937,10 +2937,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C10" t="n">
         <v>11.0</v>
@@ -2957,10 +2957,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C11" t="n">
         <v>12.0</v>
@@ -2977,10 +2977,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C12" t="n">
         <v>14.0</v>
@@ -3052,10 +3052,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C21" t="n">
         <v>8.0</v>
@@ -3147,10 +3147,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C31" t="n">
         <v>2.0</v>
@@ -3167,10 +3167,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="C32" t="n">
         <v>5.0</v>
@@ -3187,10 +3187,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C33" t="n">
         <v>6.0</v>
@@ -3207,10 +3207,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C34" t="n">
         <v>7.0</v>
@@ -3227,10 +3227,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C35" t="n">
         <v>8.0</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
         <v>130</v>
@@ -3267,7 +3267,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B37" t="s">
         <v>153</v>
@@ -3287,7 +3287,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B38" t="s">
         <v>154</v>
@@ -3465,7 +3465,7 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C52" t="n">
         <v>1.0</v>
@@ -3482,10 +3482,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B53" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C53" t="n">
         <v>12.0</v>
@@ -3502,10 +3502,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B54" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C54" t="n">
         <v>14.0</v>
@@ -3577,10 +3577,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C63" t="n">
         <v>7.0</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B64" t="s">
         <v>130</v>
@@ -3617,10 +3617,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B65" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C65" t="n">
         <v>11.0</v>
@@ -3830,7 +3830,7 @@
         <v>11</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C86" t="n">
         <v>1.0</v>
@@ -3847,10 +3847,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B87" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C87" t="n">
         <v>4.0</v>
@@ -3867,7 +3867,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B88" t="s">
         <v>130</v>
@@ -3887,10 +3887,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C89" t="n">
         <v>11.0</v>
@@ -3907,10 +3907,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B90" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C90" t="n">
         <v>13.0</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B91" t="s">
         <v>151</v>
@@ -4140,7 +4140,7 @@
         <v>11</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C112" t="n">
         <v>1.0</v>
@@ -4290,7 +4290,7 @@
         <v>11</v>
       </c>
       <c r="B130" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C130" t="n">
         <v>1.0</v>
@@ -4437,10 +4437,10 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B148" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="C148" t="n">
         <v>6.0</v>
@@ -4515,7 +4515,7 @@
         <v>11</v>
       </c>
       <c r="B157" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C157" t="n">
         <v>1.0</v>
@@ -4757,10 +4757,10 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
+        <v>80</v>
+      </c>
+      <c r="B185" t="s">
         <v>86</v>
-      </c>
-      <c r="B185" t="s">
-        <v>103</v>
       </c>
       <c r="C185" t="n">
         <v>3.0</v>
@@ -4777,10 +4777,10 @@
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B186" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C186" t="n">
         <v>12.0</v>
@@ -4797,10 +4797,10 @@
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B187" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C187" t="n">
         <v>14.0</v>
@@ -5065,7 +5065,7 @@
         <v>11</v>
       </c>
       <c r="B216" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C216" t="n">
         <v>1.0</v>
@@ -5160,7 +5160,7 @@
         <v>11</v>
       </c>
       <c r="B226" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C226" t="n">
         <v>1.0</v>
@@ -5232,10 +5232,10 @@
     </row>
     <row r="235">
       <c r="A235" t="s">
+        <v>80</v>
+      </c>
+      <c r="B235" t="s">
         <v>86</v>
-      </c>
-      <c r="B235" t="s">
-        <v>103</v>
       </c>
       <c r="C235" t="n">
         <v>3.0</v>
@@ -5252,10 +5252,10 @@
     </row>
     <row r="236">
       <c r="A236" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B236" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C236" t="n">
         <v>12.0</v>
@@ -5272,10 +5272,10 @@
     </row>
     <row r="237">
       <c r="A237" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B237" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C237" t="n">
         <v>14.0</v>
@@ -5442,10 +5442,10 @@
     </row>
     <row r="256">
       <c r="A256" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="B256" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C256" t="n">
         <v>7.0</v>
@@ -5517,7 +5517,7 @@
     </row>
     <row r="265">
       <c r="A265" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B265" t="s">
         <v>153</v>
@@ -6192,10 +6192,10 @@
     </row>
     <row r="346">
       <c r="A346" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B346" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C346" t="n">
         <v>10.0</v>
@@ -6267,7 +6267,7 @@
     </row>
     <row r="355">
       <c r="A355" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B355" t="s">
         <v>154</v>
@@ -6492,10 +6492,10 @@
     </row>
     <row r="382">
       <c r="A382" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B382" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C382" t="n">
         <v>4.0</v>
@@ -6512,10 +6512,10 @@
     </row>
     <row r="383">
       <c r="A383" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B383" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C383" t="n">
         <v>13.0</v>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="384">
       <c r="A384" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B384" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
Generate Balance de comprobacion sheet
</commit_message>
<xml_diff>
--- a/Contabilidad.xlsx
+++ b/Contabilidad.xlsx
@@ -5,14 +5,15 @@
   <sheets>
     <sheet state="visible" name="Libro Diario" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="Plan de Cuentas" sheetId="2" r:id="rId4"/>
-    <sheet name="Libro Mayor" r:id="rId5" sheetId="3"/>
+    <sheet name="Libro Mayor" r:id="rId5" sheetId="5"/>
+    <sheet name="Balance de Comprobacion" r:id="rId6" sheetId="6"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2358" uniqueCount="289">
   <si>
     <t>Libro Diario</t>
   </si>
@@ -792,6 +793,93 @@
   </si>
   <si>
     <t>Codigo: 5.2.01</t>
+  </si>
+  <si>
+    <t>Balance de comprobacion</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Cuenta</t>
+  </si>
+  <si>
+    <t>Suma Debe</t>
+  </si>
+  <si>
+    <t>Suma Haber</t>
+  </si>
+  <si>
+    <t>Saldo Debe</t>
+  </si>
+  <si>
+    <t>Saldo Haber</t>
+  </si>
+  <si>
+    <t>CAJA</t>
+  </si>
+  <si>
+    <t>INVENTARIO DE MERCADERIAS</t>
+  </si>
+  <si>
+    <t>ANTICIPO SUELDOS</t>
+  </si>
+  <si>
+    <t>MUEBLES DE OFICINA</t>
+  </si>
+  <si>
+    <t>INVERSIONES FINANCIERAS</t>
+  </si>
+  <si>
+    <t>APORTE INDIVIDUAL POR PAGAR</t>
+  </si>
+  <si>
+    <t>APORTE PATRONAL POR PAGAR</t>
+  </si>
+  <si>
+    <t>MULTAS POR PAGAR</t>
+  </si>
+  <si>
+    <t>IVA POR PAGAR</t>
+  </si>
+  <si>
+    <t>DECIMO TERCERO</t>
+  </si>
+  <si>
+    <t>DECIMO CUARTO</t>
+  </si>
+  <si>
+    <t>FONDOS DE RESERVA</t>
+  </si>
+  <si>
+    <t>APORTE PATRONAL</t>
+  </si>
+  <si>
+    <t>COMISIONES</t>
+  </si>
+  <si>
+    <t>HORAS EXTRA</t>
+  </si>
+  <si>
+    <t>TRANSPORTE Y MOVILIZACION</t>
+  </si>
+  <si>
+    <t>VIATICOS</t>
+  </si>
+  <si>
+    <t>HONORARIOS</t>
+  </si>
+  <si>
+    <t>IMPUESTOS FISCALES</t>
+  </si>
+  <si>
+    <t>COSTO DE VENTA</t>
+  </si>
+  <si>
+    <t>TOTALES</t>
   </si>
 </sst>
 </file>
@@ -851,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="132">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -895,6 +983,240 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -1033,7 +1355,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="26" customWidth="true" width="7.63" collapsed="false"/>
+    <col min="1" max="26" customWidth="true" width="7.63" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1520,7 +1842,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="26" customWidth="true" width="7.63" collapsed="false"/>
+    <col min="1" max="26" customWidth="true" width="7.63" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2792,7 +3114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2801,7 +3123,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="16">
+      <c r="A1" t="s" s="93">
         <v>175</v>
       </c>
     </row>
@@ -3016,7 +3338,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s" s="17">
+      <c r="A17" t="s" s="94">
         <v>175</v>
       </c>
     </row>
@@ -3111,7 +3433,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s" s="18">
+      <c r="A27" t="s" s="95">
         <v>175</v>
       </c>
     </row>
@@ -3426,7 +3748,7 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s" s="19">
+      <c r="A48" t="s" s="96">
         <v>175</v>
       </c>
     </row>
@@ -3541,7 +3863,7 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s" s="20">
+      <c r="A59" t="s" s="97">
         <v>175</v>
       </c>
     </row>
@@ -3716,7 +4038,7 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s" s="21">
+      <c r="A73" t="s" s="98">
         <v>175</v>
       </c>
     </row>
@@ -3791,7 +4113,7 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="s" s="22">
+      <c r="A82" t="s" s="99">
         <v>175</v>
       </c>
     </row>
@@ -4006,7 +4328,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s" s="23">
+      <c r="A98" t="s" s="100">
         <v>175</v>
       </c>
     </row>
@@ -4101,7 +4423,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="s" s="24">
+      <c r="A108" t="s" s="101">
         <v>175</v>
       </c>
     </row>
@@ -4176,7 +4498,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="s" s="25">
+      <c r="A117" t="s" s="102">
         <v>175</v>
       </c>
     </row>
@@ -4251,7 +4573,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="s" s="26">
+      <c r="A126" t="s" s="103">
         <v>175</v>
       </c>
     </row>
@@ -4326,7 +4648,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="s" s="27">
+      <c r="A135" t="s" s="104">
         <v>175</v>
       </c>
     </row>
@@ -4401,7 +4723,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="s" s="28">
+      <c r="A144" t="s" s="105">
         <v>175</v>
       </c>
     </row>
@@ -4476,7 +4798,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="s" s="29">
+      <c r="A153" t="s" s="106">
         <v>175</v>
       </c>
     </row>
@@ -4571,7 +4893,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="s" s="30">
+      <c r="A163" t="s" s="107">
         <v>175</v>
       </c>
     </row>
@@ -4646,7 +4968,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="s" s="31">
+      <c r="A172" t="s" s="108">
         <v>175</v>
       </c>
     </row>
@@ -4721,7 +5043,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="s" s="32">
+      <c r="A181" t="s" s="109">
         <v>175</v>
       </c>
     </row>
@@ -4876,7 +5198,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="s" s="33">
+      <c r="A194" t="s" s="110">
         <v>175</v>
       </c>
     </row>
@@ -4951,7 +5273,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="s" s="34">
+      <c r="A203" t="s" s="111">
         <v>175</v>
       </c>
     </row>
@@ -5026,7 +5348,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" t="s" s="35">
+      <c r="A212" t="s" s="112">
         <v>175</v>
       </c>
     </row>
@@ -5121,7 +5443,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" t="s" s="36">
+      <c r="A222" t="s" s="113">
         <v>175</v>
       </c>
     </row>
@@ -5196,7 +5518,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" t="s" s="37">
+      <c r="A231" t="s" s="114">
         <v>175</v>
       </c>
     </row>
@@ -5331,7 +5653,7 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" t="s" s="38">
+      <c r="A243" t="s" s="115">
         <v>175</v>
       </c>
     </row>
@@ -5406,7 +5728,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" t="s" s="39">
+      <c r="A252" t="s" s="116">
         <v>175</v>
       </c>
     </row>
@@ -5481,7 +5803,7 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" t="s" s="40">
+      <c r="A261" t="s" s="117">
         <v>175</v>
       </c>
     </row>
@@ -5556,7 +5878,7 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" t="s" s="41">
+      <c r="A270" t="s" s="118">
         <v>175</v>
       </c>
     </row>
@@ -5631,7 +5953,7 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" t="s" s="42">
+      <c r="A279" t="s" s="119">
         <v>175</v>
       </c>
     </row>
@@ -5706,7 +6028,7 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" t="s" s="43">
+      <c r="A288" t="s" s="120">
         <v>175</v>
       </c>
     </row>
@@ -5781,7 +6103,7 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" t="s" s="44">
+      <c r="A297" t="s" s="121">
         <v>175</v>
       </c>
     </row>
@@ -5856,7 +6178,7 @@
       </c>
     </row>
     <row r="306">
-      <c r="A306" t="s" s="45">
+      <c r="A306" t="s" s="122">
         <v>175</v>
       </c>
     </row>
@@ -5931,7 +6253,7 @@
       </c>
     </row>
     <row r="315">
-      <c r="A315" t="s" s="46">
+      <c r="A315" t="s" s="123">
         <v>175</v>
       </c>
     </row>
@@ -6006,7 +6328,7 @@
       </c>
     </row>
     <row r="324">
-      <c r="A324" t="s" s="47">
+      <c r="A324" t="s" s="124">
         <v>175</v>
       </c>
     </row>
@@ -6081,7 +6403,7 @@
       </c>
     </row>
     <row r="333">
-      <c r="A333" t="s" s="48">
+      <c r="A333" t="s" s="125">
         <v>175</v>
       </c>
     </row>
@@ -6156,7 +6478,7 @@
       </c>
     </row>
     <row r="342">
-      <c r="A342" t="s" s="49">
+      <c r="A342" t="s" s="126">
         <v>175</v>
       </c>
     </row>
@@ -6231,7 +6553,7 @@
       </c>
     </row>
     <row r="351">
-      <c r="A351" t="s" s="50">
+      <c r="A351" t="s" s="127">
         <v>175</v>
       </c>
     </row>
@@ -6306,7 +6628,7 @@
       </c>
     </row>
     <row r="360">
-      <c r="A360" t="s" s="51">
+      <c r="A360" t="s" s="128">
         <v>175</v>
       </c>
     </row>
@@ -6381,7 +6703,7 @@
       </c>
     </row>
     <row r="369">
-      <c r="A369" t="s" s="52">
+      <c r="A369" t="s" s="129">
         <v>175</v>
       </c>
     </row>
@@ -6456,7 +6778,7 @@
       </c>
     </row>
     <row r="378">
-      <c r="A378" t="s" s="53">
+      <c r="A378" t="s" s="130">
         <v>175</v>
       </c>
     </row>
@@ -6709,4 +7031,939 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="131">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" t="s">
+        <v>266</v>
+      </c>
+      <c r="G3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" t="n">
+        <v>46090.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>31810.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>14280.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>78.4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>21.599999999999994</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="n">
+        <v>66530.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>24341.04</v>
+      </c>
+      <c r="F6" t="n">
+        <v>42188.96</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="n">
+        <v>32250.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>6250.0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>26000.0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4952.4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4952.4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>269</v>
+      </c>
+      <c r="D10" t="n">
+        <v>99103.8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>32152.27</v>
+      </c>
+      <c r="F10" t="n">
+        <v>66951.53</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" t="n">
+        <v>15000.0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>15000.0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>624.94</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>624.94</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>272</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5000.0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>37100.0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>37100.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>273</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>487.78</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>487.78</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>627.15</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>627.15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="n">
+        <v>7380.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>7380.0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>275</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>276</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1857.6</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1857.6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>16500.0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>16500.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>118500.0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>118500.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" t="n">
+        <v>6250.0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>61500.0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>55250.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" t="n">
+        <v>4504.0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>4504.0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>200.0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D30" t="n">
+        <v>624.94</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>624.94</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
+        <v>277</v>
+      </c>
+      <c r="D31" t="n">
+        <v>430.14</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>430.14</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" t="s">
+        <v>278</v>
+      </c>
+      <c r="D32" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" t="s">
+        <v>279</v>
+      </c>
+      <c r="D33" t="n">
+        <v>429.97</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>429.97</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
+        <v>280</v>
+      </c>
+      <c r="D34" t="n">
+        <v>627.15</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>627.15</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>281</v>
+      </c>
+      <c r="D35" t="n">
+        <v>227.5</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>227.5</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" t="s">
+        <v>282</v>
+      </c>
+      <c r="D36" t="n">
+        <v>430.21</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>430.21</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" t="s">
+        <v>283</v>
+      </c>
+      <c r="D37" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
+        <v>284</v>
+      </c>
+      <c r="D38" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>140</v>
+      </c>
+      <c r="C39" t="s">
+        <v>285</v>
+      </c>
+      <c r="D39" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" t="s">
+        <v>286</v>
+      </c>
+      <c r="D40" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" t="s">
+        <v>287</v>
+      </c>
+      <c r="D41" t="n">
+        <v>30652.27</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3103.8</v>
+      </c>
+      <c r="F41" t="n">
+        <v>27548.47</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="s">
+        <v>288</v>
+      </c>
+      <c r="D42" t="n">
+        <v>347732.88000000006</v>
+      </c>
+      <c r="E42" t="n">
+        <v>347732.87999999995</v>
+      </c>
+      <c r="F42" t="n">
+        <v>231114.97</v>
+      </c>
+      <c r="G42" t="n">
+        <v>231114.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:H2"/>
+  </mergeCells>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>